<commit_message>
much more serious now
</commit_message>
<xml_diff>
--- a/FAA.xlsx
+++ b/FAA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\GitHub\Dave_ML\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\National Programs\Planning\Data\AircraftType\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{650D6B75-1170-4F59-BCC1-DAAB3C9F3B1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C5DE80-2351-4134-A135-D3BA839046F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="2010" windowWidth="28800" windowHeight="15345" xr2:uid="{852B0E64-BCCC-407E-85AF-9EDDBE8136BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27825" windowHeight="16440" xr2:uid="{852B0E64-BCCC-407E-85AF-9EDDBE8136BD}"/>
   </bookViews>
   <sheets>
     <sheet name="ACD_Data" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7788" uniqueCount="1413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7789" uniqueCount="1413">
   <si>
     <t>ICAO_Code</t>
   </si>
@@ -6521,9 +6521,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6561,7 +6561,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -6667,7 +6667,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6809,7 +6809,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -6817,13 +6817,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2C235D-FDEC-42F2-8FD4-154978FFF057}">
-  <dimension ref="A1:AN390"/>
+  <dimension ref="A1:BD390"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AF2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B158" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AN1" sqref="AN1:AN1048576"/>
+      <selection pane="bottomRight" activeCell="Q171" sqref="Q171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6867,10 +6867,12 @@
     <col min="38" max="38" width="22" style="49" customWidth="1"/>
     <col min="39" max="39" width="35.42578125" style="49" customWidth="1"/>
     <col min="40" max="40" width="255.7109375" style="41" bestFit="1" customWidth="1"/>
-    <col min="41" max="16384" width="9.140625" style="41"/>
+    <col min="41" max="47" width="9.140625" style="41"/>
+    <col min="48" max="48" width="52.42578125" style="41" customWidth="1"/>
+    <col min="49" max="16384" width="9.140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -6991,8 +6993,9 @@
       <c r="AN1" s="40" t="s">
         <v>39</v>
       </c>
+      <c r="AO1" s="4"/>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>40</v>
       </c>
@@ -7099,8 +7102,9 @@
         <v>33752</v>
       </c>
       <c r="AN2" s="11"/>
+      <c r="AO2" s="4"/>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>58</v>
       </c>
@@ -7207,8 +7211,9 @@
         <v>1972</v>
       </c>
       <c r="AN3" s="15"/>
+      <c r="AO3" s="4"/>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>66</v>
       </c>
@@ -7317,8 +7322,9 @@
       <c r="AN4" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO4" s="4"/>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>72</v>
       </c>
@@ -7427,8 +7433,9 @@
       <c r="AN5" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO5" s="4"/>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>76</v>
       </c>
@@ -7537,8 +7544,9 @@
       <c r="AN6" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO6" s="1"/>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>79</v>
       </c>
@@ -7647,8 +7655,9 @@
       <c r="AN7" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO7" s="4"/>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>84</v>
       </c>
@@ -7757,8 +7766,9 @@
       <c r="AN8" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO8" s="4"/>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>87</v>
       </c>
@@ -7867,8 +7877,9 @@
       <c r="AN9" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO9" s="4"/>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>90</v>
       </c>
@@ -7977,8 +7988,9 @@
       <c r="AN10" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO10" s="4"/>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>93</v>
       </c>
@@ -8089,8 +8101,9 @@
       <c r="AN11" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO11" s="4"/>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>96</v>
       </c>
@@ -8201,8 +8214,9 @@
       <c r="AN12" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO12" s="4"/>
     </row>
-    <row r="13" spans="1:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>99</v>
       </c>
@@ -8321,8 +8335,9 @@
       <c r="AN13" s="42" t="s">
         <v>102</v>
       </c>
+      <c r="AO13" s="4"/>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>103</v>
       </c>
@@ -8431,8 +8446,9 @@
       <c r="AN14" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO14" s="4"/>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>108</v>
       </c>
@@ -8541,8 +8557,9 @@
       <c r="AN15" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO15" s="4"/>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>111</v>
       </c>
@@ -8649,8 +8666,9 @@
         <v>260</v>
       </c>
       <c r="AN16" s="11"/>
+      <c r="AO16" s="4"/>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>114</v>
       </c>
@@ -8757,8 +8775,9 @@
         <v>6</v>
       </c>
       <c r="AN17" s="15"/>
+      <c r="AO17" s="4"/>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>116</v>
       </c>
@@ -8867,8 +8886,9 @@
       <c r="AN18" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO18" s="4"/>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>119</v>
       </c>
@@ -8975,8 +8995,9 @@
         <v>262</v>
       </c>
       <c r="AN19" s="15"/>
+      <c r="AO19" s="4"/>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>123</v>
       </c>
@@ -9083,8 +9104,9 @@
         <v>22390</v>
       </c>
       <c r="AN20" s="11"/>
+      <c r="AO20" s="4"/>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>126</v>
       </c>
@@ -9191,8 +9213,9 @@
         <v>158</v>
       </c>
       <c r="AN21" s="15"/>
+      <c r="AO21" s="4"/>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>130</v>
       </c>
@@ -9299,8 +9322,9 @@
         <v>3639</v>
       </c>
       <c r="AN22" s="11"/>
+      <c r="AO22" s="4"/>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>133</v>
       </c>
@@ -9409,8 +9433,9 @@
       <c r="AN23" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO23" s="4"/>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>136</v>
       </c>
@@ -9519,8 +9544,9 @@
       <c r="AN24" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO24" s="4"/>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
         <v>140</v>
       </c>
@@ -9629,8 +9655,9 @@
       <c r="AN25" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO25" s="4"/>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>145</v>
       </c>
@@ -9737,8 +9764,9 @@
         <v>2656</v>
       </c>
       <c r="AN26" s="11"/>
+      <c r="AO26" s="4"/>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
         <v>149</v>
       </c>
@@ -9845,8 +9873,9 @@
         <v>16</v>
       </c>
       <c r="AN27" s="15"/>
+      <c r="AO27" s="4"/>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>158</v>
       </c>
@@ -9953,8 +9982,12 @@
         <v>762</v>
       </c>
       <c r="AN28" s="11"/>
+      <c r="AO28" s="4"/>
+      <c r="BD28" s="41" t="s">
+        <v>162</v>
+      </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
         <v>163</v>
       </c>
@@ -10061,8 +10094,9 @@
         <v>18094</v>
       </c>
       <c r="AN29" s="15"/>
+      <c r="AO29" s="4"/>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>166</v>
       </c>
@@ -10169,8 +10203,9 @@
         <v>6632</v>
       </c>
       <c r="AN30" s="11"/>
+      <c r="AO30" s="4"/>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>170</v>
       </c>
@@ -10277,8 +10312,9 @@
         <v>34313</v>
       </c>
       <c r="AN31" s="15"/>
+      <c r="AO31" s="4"/>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>173</v>
       </c>
@@ -10385,8 +10421,9 @@
         <v>22</v>
       </c>
       <c r="AN32" s="11"/>
+      <c r="AO32" s="4"/>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
         <v>175</v>
       </c>
@@ -10493,8 +10530,9 @@
         <v>338</v>
       </c>
       <c r="AN33" s="15"/>
+      <c r="AO33" s="4"/>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>178</v>
       </c>
@@ -10601,8 +10639,9 @@
         <v>336</v>
       </c>
       <c r="AN34" s="11"/>
+      <c r="AO34" s="4"/>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>181</v>
       </c>
@@ -10709,8 +10748,9 @@
         <v>562</v>
       </c>
       <c r="AN35" s="15"/>
+      <c r="AO35" s="4"/>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>184</v>
       </c>
@@ -10817,8 +10857,9 @@
         <v>18844</v>
       </c>
       <c r="AN36" s="11"/>
+      <c r="AO36" s="4"/>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>188</v>
       </c>
@@ -10925,8 +10966,9 @@
         <v>8292</v>
       </c>
       <c r="AN37" s="15"/>
+      <c r="AO37" s="4"/>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>191</v>
       </c>
@@ -11033,8 +11075,9 @@
         <v>22564</v>
       </c>
       <c r="AN38" s="11"/>
+      <c r="AO38" s="4"/>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
         <v>195</v>
       </c>
@@ -11141,8 +11184,9 @@
         <v>2871</v>
       </c>
       <c r="AN39" s="15"/>
+      <c r="AO39" s="4"/>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>198</v>
       </c>
@@ -11249,8 +11293,9 @@
         <v>4</v>
       </c>
       <c r="AN40" s="11"/>
+      <c r="AO40" s="4"/>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
         <v>203</v>
       </c>
@@ -11357,8 +11402,9 @@
         <v>0</v>
       </c>
       <c r="AN41" s="15"/>
+      <c r="AO41" s="4"/>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>206</v>
       </c>
@@ -11465,8 +11511,9 @@
         <v>36007</v>
       </c>
       <c r="AN42" s="11"/>
+      <c r="AO42" s="4"/>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
         <v>212</v>
       </c>
@@ -11573,8 +11620,9 @@
         <v>40</v>
       </c>
       <c r="AN43" s="15"/>
+      <c r="AO43" s="4"/>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
         <v>216</v>
       </c>
@@ -11681,8 +11729,9 @@
         <v>86048</v>
       </c>
       <c r="AN44" s="11"/>
+      <c r="AO44" s="4"/>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
         <v>220</v>
       </c>
@@ -11789,8 +11838,9 @@
         <v>10</v>
       </c>
       <c r="AN45" s="15"/>
+      <c r="AO45" s="4"/>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
         <v>223</v>
       </c>
@@ -11897,8 +11947,9 @@
         <v>38632</v>
       </c>
       <c r="AN46" s="11"/>
+      <c r="AO46" s="4"/>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
         <v>225</v>
       </c>
@@ -12005,8 +12056,9 @@
         <v>46612</v>
       </c>
       <c r="AN47" s="15"/>
+      <c r="AO47" s="4"/>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
         <v>227</v>
       </c>
@@ -12113,8 +12165,9 @@
         <v>238</v>
       </c>
       <c r="AN48" s="11"/>
+      <c r="AO48" s="4"/>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A49" s="12" t="s">
         <v>230</v>
       </c>
@@ -12221,8 +12274,9 @@
         <v>2</v>
       </c>
       <c r="AN49" s="15"/>
+      <c r="AO49" s="4"/>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
         <v>233</v>
       </c>
@@ -12329,8 +12383,9 @@
         <v>80491</v>
       </c>
       <c r="AN50" s="11"/>
+      <c r="AO50" s="4"/>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A51" s="12" t="s">
         <v>236</v>
       </c>
@@ -12437,8 +12492,9 @@
         <v>11018</v>
       </c>
       <c r="AN51" s="15"/>
+      <c r="AO51" s="4"/>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
         <v>239</v>
       </c>
@@ -12545,8 +12601,9 @@
         <v>9536</v>
       </c>
       <c r="AN52" s="11"/>
+      <c r="AO52" s="4"/>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A53" s="12" t="s">
         <v>242</v>
       </c>
@@ -12653,8 +12710,9 @@
         <v>65584</v>
       </c>
       <c r="AN53" s="15"/>
+      <c r="AO53" s="4"/>
     </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
         <v>245</v>
       </c>
@@ -12761,8 +12819,9 @@
         <v>318</v>
       </c>
       <c r="AN54" s="11"/>
+      <c r="AO54" s="4"/>
     </row>
-    <row r="55" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A55" s="12" t="s">
         <v>249</v>
       </c>
@@ -12869,8 +12928,9 @@
         <v>1226</v>
       </c>
       <c r="AN55" s="15"/>
+      <c r="AO55" s="4"/>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
         <v>253</v>
       </c>
@@ -12987,8 +13047,9 @@
       <c r="AN56" s="11" t="s">
         <v>1412</v>
       </c>
+      <c r="AO56" s="4"/>
     </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
         <v>256</v>
       </c>
@@ -13095,8 +13156,9 @@
         <v>4292</v>
       </c>
       <c r="AN57" s="15"/>
+      <c r="AO57" s="4"/>
     </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
         <v>259</v>
       </c>
@@ -13203,8 +13265,9 @@
         <v>488909</v>
       </c>
       <c r="AN58" s="11"/>
+      <c r="AO58" s="4"/>
     </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A59" s="12" t="s">
         <v>262</v>
       </c>
@@ -13311,8 +13374,9 @@
         <v>1826</v>
       </c>
       <c r="AN59" s="15"/>
+      <c r="AO59" s="4"/>
     </row>
-    <row r="60" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
         <v>266</v>
       </c>
@@ -13429,8 +13493,9 @@
       <c r="AN60" s="11" t="s">
         <v>270</v>
       </c>
+      <c r="AO60" s="4"/>
     </row>
-    <row r="61" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A61" s="12" t="s">
         <v>271</v>
       </c>
@@ -13547,8 +13612,9 @@
       <c r="AN61" s="15" t="s">
         <v>270</v>
       </c>
+      <c r="AO61" s="4"/>
     </row>
-    <row r="62" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
         <v>274</v>
       </c>
@@ -13665,8 +13731,9 @@
       <c r="AN62" s="11" t="s">
         <v>270</v>
       </c>
+      <c r="AO62" s="4"/>
     </row>
-    <row r="63" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A63" s="12" t="s">
         <v>277</v>
       </c>
@@ -13773,8 +13840,9 @@
         <v>522</v>
       </c>
       <c r="AN63" s="15"/>
+      <c r="AO63" s="4"/>
     </row>
-    <row r="64" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
         <v>281</v>
       </c>
@@ -13881,8 +13949,9 @@
         <v>568</v>
       </c>
       <c r="AN64" s="11"/>
+      <c r="AO64" s="4"/>
     </row>
-    <row r="65" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A65" s="12" t="s">
         <v>284</v>
       </c>
@@ -13989,8 +14058,9 @@
         <v>9641</v>
       </c>
       <c r="AN65" s="15"/>
+      <c r="AO65" s="4"/>
     </row>
-    <row r="66" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
         <v>287</v>
       </c>
@@ -14097,8 +14167,9 @@
         <v>2976</v>
       </c>
       <c r="AN66" s="11"/>
+      <c r="AO66" s="4"/>
     </row>
-    <row r="67" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A67" s="12" t="s">
         <v>290</v>
       </c>
@@ -14207,8 +14278,9 @@
       <c r="AN67" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO67" s="4"/>
     </row>
-    <row r="68" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
         <v>293</v>
       </c>
@@ -14315,8 +14387,9 @@
         <v>28</v>
       </c>
       <c r="AN68" s="11"/>
+      <c r="AO68" s="4"/>
     </row>
-    <row r="69" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A69" s="12" t="s">
         <v>296</v>
       </c>
@@ -14425,8 +14498,9 @@
         <v>15444</v>
       </c>
       <c r="AN69" s="15"/>
+      <c r="AO69" s="4"/>
     </row>
-    <row r="70" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
         <v>299</v>
       </c>
@@ -14535,8 +14609,9 @@
       <c r="AN70" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO70" s="4"/>
     </row>
-    <row r="71" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A71" s="12" t="s">
         <v>302</v>
       </c>
@@ -14647,8 +14722,9 @@
       <c r="AN71" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO71" s="4"/>
     </row>
-    <row r="72" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
         <v>305</v>
       </c>
@@ -14757,8 +14833,9 @@
       <c r="AN72" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO72" s="4"/>
     </row>
-    <row r="73" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A73" s="12" t="s">
         <v>308</v>
       </c>
@@ -14867,8 +14944,9 @@
       <c r="AN73" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO73" s="4"/>
     </row>
-    <row r="74" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
         <v>311</v>
       </c>
@@ -14979,8 +15057,9 @@
       <c r="AN74" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO74" s="4"/>
     </row>
-    <row r="75" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A75" s="12" t="s">
         <v>314</v>
       </c>
@@ -15091,8 +15170,9 @@
       <c r="AN75" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO75" s="4"/>
     </row>
-    <row r="76" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
         <v>317</v>
       </c>
@@ -15211,8 +15291,9 @@
       <c r="AN76" s="11" t="s">
         <v>270</v>
       </c>
+      <c r="AO76" s="4"/>
     </row>
-    <row r="77" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A77" s="12" t="s">
         <v>320</v>
       </c>
@@ -15331,8 +15412,9 @@
       <c r="AN77" s="15" t="s">
         <v>270</v>
       </c>
+      <c r="AO77" s="4"/>
     </row>
-    <row r="78" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
         <v>323</v>
       </c>
@@ -15439,8 +15521,9 @@
         <v>22</v>
       </c>
       <c r="AN78" s="11"/>
+      <c r="AO78" s="4"/>
     </row>
-    <row r="79" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A79" s="12" t="s">
         <v>326</v>
       </c>
@@ -15547,8 +15630,9 @@
         <v>2222</v>
       </c>
       <c r="AN79" s="15"/>
+      <c r="AO79" s="4"/>
     </row>
-    <row r="80" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
         <v>329</v>
       </c>
@@ -15655,8 +15739,9 @@
         <v>10</v>
       </c>
       <c r="AN80" s="11"/>
+      <c r="AO80" s="4"/>
     </row>
-    <row r="81" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A81" s="12" t="s">
         <v>332</v>
       </c>
@@ -15765,8 +15850,9 @@
       <c r="AN81" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO81" s="4"/>
     </row>
-    <row r="82" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
         <v>335</v>
       </c>
@@ -15875,8 +15961,9 @@
       <c r="AN82" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO82" s="4"/>
     </row>
-    <row r="83" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A83" s="12" t="s">
         <v>338</v>
       </c>
@@ -15985,8 +16072,9 @@
         <v>815959</v>
       </c>
       <c r="AN83" s="15"/>
+      <c r="AO83" s="4"/>
     </row>
-    <row r="84" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
         <v>341</v>
       </c>
@@ -16095,8 +16183,9 @@
         <v>109218</v>
       </c>
       <c r="AN84" s="11"/>
+      <c r="AO84" s="4"/>
     </row>
-    <row r="85" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A85" s="12" t="s">
         <v>344</v>
       </c>
@@ -16203,8 +16292,9 @@
         <v>107137</v>
       </c>
       <c r="AN85" s="15"/>
+      <c r="AO85" s="4"/>
     </row>
-    <row r="86" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
         <v>347</v>
       </c>
@@ -16313,8 +16403,9 @@
         <v>960856</v>
       </c>
       <c r="AN86" s="11"/>
+      <c r="AO86" s="4"/>
     </row>
-    <row r="87" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A87" s="12" t="s">
         <v>350</v>
       </c>
@@ -16421,8 +16512,9 @@
         <v>60793</v>
       </c>
       <c r="AN87" s="15"/>
+      <c r="AO87" s="4"/>
     </row>
-    <row r="88" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
         <v>353</v>
       </c>
@@ -16531,8 +16623,9 @@
       <c r="AN88" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO88" s="4"/>
     </row>
-    <row r="89" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A89" s="12" t="s">
         <v>356</v>
       </c>
@@ -16641,8 +16734,9 @@
       <c r="AN89" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO89" s="4"/>
     </row>
-    <row r="90" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
         <v>359</v>
       </c>
@@ -16751,8 +16845,9 @@
       <c r="AN90" s="11" t="s">
         <v>1410</v>
       </c>
+      <c r="AO90" s="4"/>
     </row>
-    <row r="91" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
         <v>362</v>
       </c>
@@ -16861,8 +16956,9 @@
       <c r="AN91" s="11" t="s">
         <v>1410</v>
       </c>
+      <c r="AO91" s="4"/>
     </row>
-    <row r="92" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
         <v>364</v>
       </c>
@@ -16971,8 +17067,9 @@
       <c r="AN92" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO92" s="4"/>
     </row>
-    <row r="93" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
         <v>367</v>
       </c>
@@ -17081,8 +17178,9 @@
       <c r="AN93" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO93" s="4"/>
     </row>
-    <row r="94" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
         <v>370</v>
       </c>
@@ -17199,8 +17297,9 @@
       <c r="AN94" s="11" t="s">
         <v>373</v>
       </c>
+      <c r="AO94" s="4"/>
     </row>
-    <row r="95" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A95" s="12" t="s">
         <v>374</v>
       </c>
@@ -17317,8 +17416,9 @@
       <c r="AN95" s="15" t="s">
         <v>373</v>
       </c>
+      <c r="AO95" s="4"/>
     </row>
-    <row r="96" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
         <v>377</v>
       </c>
@@ -17427,8 +17527,9 @@
       <c r="AN96" s="11" t="s">
         <v>380</v>
       </c>
+      <c r="AO96" s="4"/>
     </row>
-    <row r="97" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
         <v>381</v>
       </c>
@@ -17535,8 +17636,9 @@
         <v>0</v>
       </c>
       <c r="AN97" s="15"/>
+      <c r="AO97" s="4"/>
     </row>
-    <row r="98" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
         <v>385</v>
       </c>
@@ -17645,8 +17747,9 @@
       <c r="AN98" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO98" s="4"/>
     </row>
-    <row r="99" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
         <v>389</v>
       </c>
@@ -17753,8 +17856,9 @@
         <v>163166</v>
       </c>
       <c r="AN99" s="15"/>
+      <c r="AO99" s="4"/>
     </row>
-    <row r="100" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
         <v>392</v>
       </c>
@@ -17861,8 +17965,9 @@
         <v>87014</v>
       </c>
       <c r="AN100" s="11"/>
+      <c r="AO100" s="4"/>
     </row>
-    <row r="101" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
         <v>395</v>
       </c>
@@ -17969,8 +18074,9 @@
         <v>1032</v>
       </c>
       <c r="AN101" s="15"/>
+      <c r="AO101" s="4"/>
     </row>
-    <row r="102" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
         <v>398</v>
       </c>
@@ -18077,8 +18183,9 @@
         <v>540</v>
       </c>
       <c r="AN102" s="11"/>
+      <c r="AO102" s="4"/>
     </row>
-    <row r="103" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
         <v>401</v>
       </c>
@@ -18187,8 +18294,9 @@
       <c r="AN103" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO103" s="4"/>
     </row>
-    <row r="104" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
         <v>404</v>
       </c>
@@ -18295,8 +18403,9 @@
         <v>6055</v>
       </c>
       <c r="AN104" s="11"/>
+      <c r="AO104" s="4"/>
     </row>
-    <row r="105" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A105" s="12" t="s">
         <v>407</v>
       </c>
@@ -18403,8 +18512,9 @@
         <v>4687</v>
       </c>
       <c r="AN105" s="15"/>
+      <c r="AO105" s="4"/>
     </row>
-    <row r="106" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
         <v>409</v>
       </c>
@@ -18513,8 +18623,9 @@
       <c r="AN106" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO106" s="4"/>
     </row>
-    <row r="107" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A107" s="12" t="s">
         <v>413</v>
       </c>
@@ -18621,8 +18732,9 @@
         <v>58462</v>
       </c>
       <c r="AN107" s="15"/>
+      <c r="AO107" s="4"/>
     </row>
-    <row r="108" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
         <v>416</v>
       </c>
@@ -18729,8 +18841,9 @@
         <v>79943</v>
       </c>
       <c r="AN108" s="11"/>
+      <c r="AO108" s="4"/>
     </row>
-    <row r="109" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
         <v>419</v>
       </c>
@@ -18837,8 +18950,9 @@
         <v>184714</v>
       </c>
       <c r="AN109" s="15"/>
+      <c r="AO109" s="4"/>
     </row>
-    <row r="110" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
         <v>422</v>
       </c>
@@ -18945,8 +19059,9 @@
         <v>425535</v>
       </c>
       <c r="AN110" s="11"/>
+      <c r="AO110" s="4"/>
     </row>
-    <row r="111" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A111" s="12" t="s">
         <v>426</v>
       </c>
@@ -19053,8 +19168,9 @@
         <v>1549</v>
       </c>
       <c r="AN111" s="15"/>
+      <c r="AO111" s="4"/>
     </row>
-    <row r="112" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
         <v>429</v>
       </c>
@@ -19161,8 +19277,9 @@
         <v>56837</v>
       </c>
       <c r="AN112" s="11"/>
+      <c r="AO112" s="4"/>
     </row>
-    <row r="113" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A113" s="12" t="s">
         <v>432</v>
       </c>
@@ -19269,8 +19386,9 @@
         <v>177473</v>
       </c>
       <c r="AN113" s="15"/>
+      <c r="AO113" s="4"/>
     </row>
-    <row r="114" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
         <v>435</v>
       </c>
@@ -19377,8 +19495,9 @@
         <v>8858</v>
       </c>
       <c r="AN114" s="11"/>
+      <c r="AO114" s="4"/>
     </row>
-    <row r="115" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A115" s="12" t="s">
         <v>437</v>
       </c>
@@ -19485,8 +19604,9 @@
         <v>18637</v>
       </c>
       <c r="AN115" s="15"/>
+      <c r="AO115" s="4"/>
     </row>
-    <row r="116" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
         <v>439</v>
       </c>
@@ -19593,8 +19713,9 @@
         <v>2</v>
       </c>
       <c r="AN116" s="11"/>
+      <c r="AO116" s="4"/>
     </row>
-    <row r="117" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A117" s="12" t="s">
         <v>441</v>
       </c>
@@ -19701,8 +19822,9 @@
         <v>5934</v>
       </c>
       <c r="AN117" s="15"/>
+      <c r="AO117" s="4"/>
     </row>
-    <row r="118" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>444</v>
       </c>
@@ -19809,8 +19931,9 @@
         <v>84</v>
       </c>
       <c r="AN118" s="11"/>
+      <c r="AO118" s="4"/>
     </row>
-    <row r="119" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A119" s="12" t="s">
         <v>446</v>
       </c>
@@ -19917,8 +20040,9 @@
         <v>1140</v>
       </c>
       <c r="AN119" s="15"/>
+      <c r="AO119" s="4"/>
     </row>
-    <row r="120" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
         <v>449</v>
       </c>
@@ -20025,8 +20149,9 @@
         <v>5346</v>
       </c>
       <c r="AN120" s="11"/>
+      <c r="AO120" s="4"/>
     </row>
-    <row r="121" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A121" s="12" t="s">
         <v>452</v>
       </c>
@@ -20133,8 +20258,9 @@
         <v>131129</v>
       </c>
       <c r="AN121" s="15"/>
+      <c r="AO121" s="4"/>
     </row>
-    <row r="122" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
         <v>455</v>
       </c>
@@ -20241,8 +20367,9 @@
         <v>470799</v>
       </c>
       <c r="AN122" s="11"/>
+      <c r="AO122" s="4"/>
     </row>
-    <row r="123" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A123" s="12" t="s">
         <v>458</v>
       </c>
@@ -20349,8 +20476,9 @@
         <v>29663</v>
       </c>
       <c r="AN123" s="15"/>
+      <c r="AO123" s="4"/>
     </row>
-    <row r="124" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
         <v>461</v>
       </c>
@@ -20457,8 +20585,9 @@
         <v>4052</v>
       </c>
       <c r="AN124" s="11"/>
+      <c r="AO124" s="4"/>
     </row>
-    <row r="125" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A125" s="12" t="s">
         <v>465</v>
       </c>
@@ -20565,8 +20694,9 @@
         <v>318</v>
       </c>
       <c r="AN125" s="15"/>
+      <c r="AO125" s="4"/>
     </row>
-    <row r="126" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
         <v>467</v>
       </c>
@@ -20673,8 +20803,9 @@
         <v>1221</v>
       </c>
       <c r="AN126" s="11"/>
+      <c r="AO126" s="4"/>
     </row>
-    <row r="127" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A127" s="12" t="s">
         <v>469</v>
       </c>
@@ -20781,8 +20912,9 @@
         <v>13046</v>
       </c>
       <c r="AN127" s="15"/>
+      <c r="AO127" s="4"/>
     </row>
-    <row r="128" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A128" s="6" t="s">
         <v>472</v>
       </c>
@@ -20889,8 +21021,9 @@
         <v>6</v>
       </c>
       <c r="AN128" s="11"/>
+      <c r="AO128" s="4"/>
     </row>
-    <row r="129" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A129" s="12" t="s">
         <v>475</v>
       </c>
@@ -20997,8 +21130,9 @@
         <v>87047</v>
       </c>
       <c r="AN129" s="15"/>
+      <c r="AO129" s="4"/>
     </row>
-    <row r="130" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A130" s="6" t="s">
         <v>479</v>
       </c>
@@ -21105,8 +21239,9 @@
         <v>24</v>
       </c>
       <c r="AN130" s="11"/>
+      <c r="AO130" s="4"/>
     </row>
-    <row r="131" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A131" s="12" t="s">
         <v>481</v>
       </c>
@@ -21213,8 +21348,9 @@
         <v>7524</v>
       </c>
       <c r="AN131" s="15"/>
+      <c r="AO131" s="4"/>
     </row>
-    <row r="132" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A132" s="6" t="s">
         <v>483</v>
       </c>
@@ -21321,8 +21457,9 @@
         <v>8425</v>
       </c>
       <c r="AN132" s="11"/>
+      <c r="AO132" s="4"/>
     </row>
-    <row r="133" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A133" s="12" t="s">
         <v>485</v>
       </c>
@@ -21429,8 +21566,9 @@
         <v>118</v>
       </c>
       <c r="AN133" s="15"/>
+      <c r="AO133" s="4"/>
     </row>
-    <row r="134" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A134" s="6" t="s">
         <v>489</v>
       </c>
@@ -21537,8 +21675,9 @@
         <v>96</v>
       </c>
       <c r="AN134" s="11"/>
+      <c r="AO134" s="4"/>
     </row>
-    <row r="135" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A135" s="12" t="s">
         <v>492</v>
       </c>
@@ -21645,8 +21784,9 @@
         <v>110263</v>
       </c>
       <c r="AN135" s="15"/>
+      <c r="AO135" s="4"/>
     </row>
-    <row r="136" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A136" s="6" t="s">
         <v>496</v>
       </c>
@@ -21753,8 +21893,9 @@
         <v>562</v>
       </c>
       <c r="AN136" s="11"/>
+      <c r="AO136" s="4"/>
     </row>
-    <row r="137" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A137" s="12" t="s">
         <v>498</v>
       </c>
@@ -21861,8 +22002,9 @@
         <v>640671</v>
       </c>
       <c r="AN137" s="15"/>
+      <c r="AO137" s="4"/>
     </row>
-    <row r="138" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A138" s="6" t="s">
         <v>501</v>
       </c>
@@ -21969,8 +22111,9 @@
         <v>486</v>
       </c>
       <c r="AN138" s="11"/>
+      <c r="AO138" s="4"/>
     </row>
-    <row r="139" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A139" s="12" t="s">
         <v>504</v>
       </c>
@@ -22077,8 +22220,9 @@
         <v>12700</v>
       </c>
       <c r="AN139" s="15"/>
+      <c r="AO139" s="4"/>
     </row>
-    <row r="140" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A140" s="6" t="s">
         <v>506</v>
       </c>
@@ -22185,8 +22329,9 @@
         <v>5140</v>
       </c>
       <c r="AN140" s="11"/>
+      <c r="AO140" s="4"/>
     </row>
-    <row r="141" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A141" s="12" t="s">
         <v>509</v>
       </c>
@@ -22293,8 +22438,9 @@
         <v>196818</v>
       </c>
       <c r="AN141" s="15"/>
+      <c r="AO141" s="4"/>
     </row>
-    <row r="142" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A142" s="6" t="s">
         <v>512</v>
       </c>
@@ -22401,8 +22547,9 @@
         <v>4732</v>
       </c>
       <c r="AN142" s="11"/>
+      <c r="AO142" s="4"/>
     </row>
-    <row r="143" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A143" s="12" t="s">
         <v>514</v>
       </c>
@@ -22509,8 +22656,9 @@
         <v>2</v>
       </c>
       <c r="AN143" s="15"/>
+      <c r="AO143" s="4"/>
     </row>
-    <row r="144" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A144" s="6" t="s">
         <v>517</v>
       </c>
@@ -22617,8 +22765,9 @@
         <v>926</v>
       </c>
       <c r="AN144" s="11"/>
+      <c r="AO144" s="4"/>
     </row>
-    <row r="145" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A145" s="12" t="s">
         <v>519</v>
       </c>
@@ -22725,8 +22874,9 @@
         <v>32900</v>
       </c>
       <c r="AN145" s="15"/>
+      <c r="AO145" s="4"/>
     </row>
-    <row r="146" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A146" s="6" t="s">
         <v>522</v>
       </c>
@@ -22833,8 +22983,9 @@
         <v>530</v>
       </c>
       <c r="AN146" s="11"/>
+      <c r="AO146" s="4"/>
     </row>
-    <row r="147" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A147" s="12" t="s">
         <v>526</v>
       </c>
@@ -22941,8 +23092,9 @@
         <v>844895</v>
       </c>
       <c r="AN147" s="15"/>
+      <c r="AO147" s="4"/>
     </row>
-    <row r="148" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A148" s="6" t="s">
         <v>529</v>
       </c>
@@ -23049,8 +23201,9 @@
         <v>43402</v>
       </c>
       <c r="AN148" s="11"/>
+      <c r="AO148" s="4"/>
     </row>
-    <row r="149" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A149" s="12" t="s">
         <v>532</v>
       </c>
@@ -23157,8 +23310,9 @@
         <v>9222</v>
       </c>
       <c r="AN149" s="15"/>
+      <c r="AO149" s="4"/>
     </row>
-    <row r="150" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A150" s="6" t="s">
         <v>536</v>
       </c>
@@ -23265,8 +23419,9 @@
         <v>10255</v>
       </c>
       <c r="AN150" s="11"/>
+      <c r="AO150" s="4"/>
     </row>
-    <row r="151" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A151" s="12" t="s">
         <v>539</v>
       </c>
@@ -23375,8 +23530,9 @@
       <c r="AN151" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO151" s="4"/>
     </row>
-    <row r="152" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A152" s="6" t="s">
         <v>542</v>
       </c>
@@ -23485,8 +23641,9 @@
       <c r="AN152" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO152" s="4"/>
     </row>
-    <row r="153" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A153" s="12" t="s">
         <v>544</v>
       </c>
@@ -23595,8 +23752,9 @@
       <c r="AN153" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO153" s="4"/>
     </row>
-    <row r="154" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A154" s="6" t="s">
         <v>546</v>
       </c>
@@ -23705,8 +23863,9 @@
       <c r="AN154" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO154" s="4"/>
     </row>
-    <row r="155" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A155" s="12" t="s">
         <v>549</v>
       </c>
@@ -23813,8 +23972,9 @@
         <v>2050</v>
       </c>
       <c r="AN155" s="15"/>
+      <c r="AO155" s="4"/>
     </row>
-    <row r="156" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A156" s="6" t="s">
         <v>552</v>
       </c>
@@ -23921,8 +24081,9 @@
         <v>82981</v>
       </c>
       <c r="AN156" s="11"/>
+      <c r="AO156" s="4"/>
     </row>
-    <row r="157" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A157" s="12" t="s">
         <v>556</v>
       </c>
@@ -24029,8 +24190,9 @@
         <v>66128</v>
       </c>
       <c r="AN157" s="15"/>
+      <c r="AO157" s="4"/>
     </row>
-    <row r="158" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A158" s="6" t="s">
         <v>559</v>
       </c>
@@ -24137,8 +24299,9 @@
         <v>800</v>
       </c>
       <c r="AN158" s="11"/>
+      <c r="AO158" s="4"/>
     </row>
-    <row r="159" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A159" s="12" t="s">
         <v>561</v>
       </c>
@@ -24245,8 +24408,9 @@
         <v>1350</v>
       </c>
       <c r="AN159" s="15"/>
+      <c r="AO159" s="4"/>
     </row>
-    <row r="160" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A160" s="6" t="s">
         <v>563</v>
       </c>
@@ -24353,8 +24517,9 @@
         <v>54531</v>
       </c>
       <c r="AN160" s="11"/>
+      <c r="AO160" s="4"/>
     </row>
-    <row r="161" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A161" s="12" t="s">
         <v>566</v>
       </c>
@@ -24461,8 +24626,9 @@
         <v>157498</v>
       </c>
       <c r="AN161" s="15"/>
+      <c r="AO161" s="4"/>
     </row>
-    <row r="162" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A162" s="6" t="s">
         <v>569</v>
       </c>
@@ -24569,8 +24735,9 @@
         <v>6144</v>
       </c>
       <c r="AN162" s="11"/>
+      <c r="AO162" s="4"/>
     </row>
-    <row r="163" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A163" s="12" t="s">
         <v>571</v>
       </c>
@@ -24677,8 +24844,9 @@
         <v>74138</v>
       </c>
       <c r="AN163" s="15"/>
+      <c r="AO163" s="4"/>
     </row>
-    <row r="164" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A164" s="6" t="s">
         <v>574</v>
       </c>
@@ -24785,8 +24953,9 @@
         <v>63712</v>
       </c>
       <c r="AN164" s="11"/>
+      <c r="AO164" s="4"/>
     </row>
-    <row r="165" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A165" s="12" t="s">
         <v>577</v>
       </c>
@@ -24893,8 +25062,9 @@
         <v>32764</v>
       </c>
       <c r="AN165" s="15"/>
+      <c r="AO165" s="4"/>
     </row>
-    <row r="166" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A166" s="6" t="s">
         <v>579</v>
       </c>
@@ -25001,8 +25171,9 @@
         <v>55820</v>
       </c>
       <c r="AN166" s="11"/>
+      <c r="AO166" s="4"/>
     </row>
-    <row r="167" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A167" s="12" t="s">
         <v>582</v>
       </c>
@@ -25111,8 +25282,9 @@
       <c r="AN167" s="15" t="s">
         <v>585</v>
       </c>
+      <c r="AO167" s="4"/>
     </row>
-    <row r="168" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A168" s="6" t="s">
         <v>586</v>
       </c>
@@ -25221,8 +25393,9 @@
       <c r="AN168" s="11" t="s">
         <v>585</v>
       </c>
+      <c r="AO168" s="4"/>
     </row>
-    <row r="169" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A169" s="12" t="s">
         <v>589</v>
       </c>
@@ -25331,8 +25504,9 @@
       <c r="AN169" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO169" s="4"/>
     </row>
-    <row r="170" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A170" s="6" t="s">
         <v>591</v>
       </c>
@@ -25441,8 +25615,9 @@
       <c r="AN170" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO170" s="4"/>
     </row>
-    <row r="171" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A171" s="12" t="s">
         <v>594</v>
       </c>
@@ -25549,8 +25724,9 @@
         <v>244</v>
       </c>
       <c r="AN171" s="15"/>
+      <c r="AO171" s="4"/>
     </row>
-    <row r="172" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A172" s="6" t="s">
         <v>596</v>
       </c>
@@ -25659,8 +25835,9 @@
       <c r="AN172" s="11" t="s">
         <v>599</v>
       </c>
+      <c r="AO172" s="4"/>
     </row>
-    <row r="173" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A173" s="12" t="s">
         <v>600</v>
       </c>
@@ -25769,8 +25946,9 @@
       <c r="AN173" s="45" t="s">
         <v>602</v>
       </c>
+      <c r="AO173" s="4"/>
     </row>
-    <row r="174" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A174" s="6" t="s">
         <v>603</v>
       </c>
@@ -25877,8 +26055,9 @@
         <v>41802</v>
       </c>
       <c r="AN174" s="11"/>
+      <c r="AO174" s="4"/>
     </row>
-    <row r="175" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A175" s="12" t="s">
         <v>605</v>
       </c>
@@ -25987,8 +26166,9 @@
       <c r="AN175" s="45" t="s">
         <v>602</v>
       </c>
+      <c r="AO175" s="4"/>
     </row>
-    <row r="176" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A176" s="6" t="s">
         <v>608</v>
       </c>
@@ -26097,8 +26277,9 @@
       <c r="AN176" s="45" t="s">
         <v>602</v>
       </c>
+      <c r="AO176" s="4"/>
     </row>
-    <row r="177" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A177" s="12" t="s">
         <v>611</v>
       </c>
@@ -26205,8 +26386,9 @@
         <v>100762</v>
       </c>
       <c r="AN177" s="15"/>
+      <c r="AO177" s="4"/>
     </row>
-    <row r="178" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A178" s="6" t="s">
         <v>614</v>
       </c>
@@ -26315,8 +26497,9 @@
       <c r="AN178" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO178" s="4"/>
     </row>
-    <row r="179" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A179" s="12" t="s">
         <v>616</v>
       </c>
@@ -26425,8 +26608,9 @@
       <c r="AN179" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO179" s="4"/>
     </row>
-    <row r="180" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A180" s="6" t="s">
         <v>619</v>
       </c>
@@ -26535,8 +26719,9 @@
       <c r="AN180" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO180" s="4"/>
     </row>
-    <row r="181" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A181" s="12" t="s">
         <v>621</v>
       </c>
@@ -26643,8 +26828,9 @@
         <v>6904</v>
       </c>
       <c r="AN181" s="15"/>
+      <c r="AO181" s="4"/>
     </row>
-    <row r="182" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A182" s="6" t="s">
         <v>623</v>
       </c>
@@ -26753,8 +26939,9 @@
       <c r="AN182" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO182" s="4"/>
     </row>
-    <row r="183" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A183" s="12" t="s">
         <v>625</v>
       </c>
@@ -26861,8 +27048,9 @@
         <v>8718</v>
       </c>
       <c r="AN183" s="15"/>
+      <c r="AO183" s="4"/>
     </row>
-    <row r="184" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A184" s="6" t="s">
         <v>628</v>
       </c>
@@ -26969,8 +27157,9 @@
         <v>14290</v>
       </c>
       <c r="AN184" s="11"/>
+      <c r="AO184" s="4"/>
     </row>
-    <row r="185" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A185" s="12" t="s">
         <v>631</v>
       </c>
@@ -27077,8 +27266,9 @@
         <v>28</v>
       </c>
       <c r="AN185" s="15"/>
+      <c r="AO185" s="4"/>
     </row>
-    <row r="186" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A186" s="6" t="s">
         <v>634</v>
       </c>
@@ -27185,8 +27375,9 @@
         <v>152</v>
       </c>
       <c r="AN186" s="11"/>
+      <c r="AO186" s="4"/>
     </row>
-    <row r="187" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A187" s="12" t="s">
         <v>637</v>
       </c>
@@ -27295,8 +27486,9 @@
       <c r="AN187" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO187" s="4"/>
     </row>
-    <row r="188" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A188" s="6" t="s">
         <v>641</v>
       </c>
@@ -27405,8 +27597,9 @@
       <c r="AN188" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO188" s="4"/>
     </row>
-    <row r="189" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A189" s="12" t="s">
         <v>643</v>
       </c>
@@ -27513,8 +27706,9 @@
         <v>900</v>
       </c>
       <c r="AN189" s="15"/>
+      <c r="AO189" s="4"/>
     </row>
-    <row r="190" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A190" s="6" t="s">
         <v>647</v>
       </c>
@@ -27623,8 +27817,9 @@
       <c r="AN190" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO190" s="4"/>
     </row>
-    <row r="191" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A191" s="12" t="s">
         <v>650</v>
       </c>
@@ -27733,8 +27928,9 @@
       <c r="AN191" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO191" s="4"/>
     </row>
-    <row r="192" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A192" s="6" t="s">
         <v>652</v>
       </c>
@@ -27841,8 +28037,9 @@
         <v>9964</v>
       </c>
       <c r="AN192" s="11"/>
+      <c r="AO192" s="4"/>
     </row>
-    <row r="193" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A193" s="12" t="s">
         <v>656</v>
       </c>
@@ -27949,8 +28146,9 @@
         <v>29710</v>
       </c>
       <c r="AN193" s="15"/>
+      <c r="AO193" s="4"/>
     </row>
-    <row r="194" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A194" s="6" t="s">
         <v>659</v>
       </c>
@@ -28057,8 +28255,9 @@
         <v>160</v>
       </c>
       <c r="AN194" s="11"/>
+      <c r="AO194" s="4"/>
     </row>
-    <row r="195" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A195" s="12" t="s">
         <v>663</v>
       </c>
@@ -28167,8 +28366,9 @@
       <c r="AN195" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO195" s="4"/>
     </row>
-    <row r="196" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A196" s="6" t="s">
         <v>666</v>
       </c>
@@ -28277,8 +28477,9 @@
       <c r="AN196" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO196" s="4"/>
     </row>
-    <row r="197" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A197" s="12" t="s">
         <v>669</v>
       </c>
@@ -28387,8 +28588,9 @@
       <c r="AN197" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO197" s="4"/>
     </row>
-    <row r="198" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A198" s="6" t="s">
         <v>672</v>
       </c>
@@ -28505,8 +28707,9 @@
       <c r="AN198" s="11" t="s">
         <v>675</v>
       </c>
+      <c r="AO198" s="4"/>
     </row>
-    <row r="199" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A199" s="12" t="s">
         <v>676</v>
       </c>
@@ -28613,8 +28816,9 @@
         <v>516</v>
       </c>
       <c r="AN199" s="15"/>
+      <c r="AO199" s="4"/>
     </row>
-    <row r="200" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A200" s="6" t="s">
         <v>679</v>
       </c>
@@ -28721,8 +28925,9 @@
         <v>2508</v>
       </c>
       <c r="AN200" s="11"/>
+      <c r="AO200" s="4"/>
     </row>
-    <row r="201" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A201" s="12" t="s">
         <v>683</v>
       </c>
@@ -28829,8 +29034,9 @@
         <v>21004</v>
       </c>
       <c r="AN201" s="15"/>
+      <c r="AO201" s="4"/>
     </row>
-    <row r="202" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A202" s="6" t="s">
         <v>687</v>
       </c>
@@ -28939,8 +29145,9 @@
       <c r="AN202" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO202" s="4"/>
     </row>
-    <row r="203" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A203" s="12" t="s">
         <v>691</v>
       </c>
@@ -29047,8 +29254,9 @@
         <v>92275</v>
       </c>
       <c r="AN203" s="15"/>
+      <c r="AO203" s="4"/>
     </row>
-    <row r="204" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A204" s="6" t="s">
         <v>695</v>
       </c>
@@ -29155,8 +29363,9 @@
         <v>23039</v>
       </c>
       <c r="AN204" s="11"/>
+      <c r="AO204" s="4"/>
     </row>
-    <row r="205" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A205" s="12" t="s">
         <v>698</v>
       </c>
@@ -29263,8 +29472,9 @@
         <v>37839</v>
       </c>
       <c r="AN205" s="15"/>
+      <c r="AO205" s="4"/>
     </row>
-    <row r="206" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A206" s="6" t="s">
         <v>702</v>
       </c>
@@ -29373,8 +29583,9 @@
       <c r="AN206" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO206" s="4"/>
     </row>
-    <row r="207" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A207" s="12" t="s">
         <v>706</v>
       </c>
@@ -29483,8 +29694,9 @@
       <c r="AN207" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO207" s="4"/>
     </row>
-    <row r="208" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A208" s="6" t="s">
         <v>709</v>
       </c>
@@ -29591,8 +29803,9 @@
         <v>4386</v>
       </c>
       <c r="AN208" s="11"/>
+      <c r="AO208" s="4"/>
     </row>
-    <row r="209" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A209" s="12" t="s">
         <v>712</v>
       </c>
@@ -29699,8 +29912,9 @@
         <v>2626</v>
       </c>
       <c r="AN209" s="15"/>
+      <c r="AO209" s="4"/>
     </row>
-    <row r="210" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A210" s="6" t="s">
         <v>715</v>
       </c>
@@ -29809,8 +30023,9 @@
       <c r="AN210" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO210" s="4"/>
     </row>
-    <row r="211" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A211" s="12" t="s">
         <v>718</v>
       </c>
@@ -29919,8 +30134,9 @@
       <c r="AN211" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO211" s="4"/>
     </row>
-    <row r="212" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A212" s="6" t="s">
         <v>721</v>
       </c>
@@ -30029,8 +30245,9 @@
       <c r="AN212" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO212" s="4"/>
     </row>
-    <row r="213" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A213" s="12" t="s">
         <v>724</v>
       </c>
@@ -30139,8 +30356,9 @@
       <c r="AN213" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO213" s="4"/>
     </row>
-    <row r="214" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A214" s="6" t="s">
         <v>728</v>
       </c>
@@ -30249,8 +30467,9 @@
       <c r="AN214" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO214" s="4"/>
     </row>
-    <row r="215" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A215" s="12" t="s">
         <v>731</v>
       </c>
@@ -30359,8 +30578,9 @@
       <c r="AN215" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO215" s="4"/>
     </row>
-    <row r="216" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A216" s="6" t="s">
         <v>734</v>
       </c>
@@ -30469,8 +30689,9 @@
       <c r="AN216" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO216" s="4"/>
     </row>
-    <row r="217" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A217" s="12" t="s">
         <v>737</v>
       </c>
@@ -30577,8 +30798,9 @@
         <v>336</v>
       </c>
       <c r="AN217" s="15"/>
+      <c r="AO217" s="4"/>
     </row>
-    <row r="218" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A218" s="6" t="s">
         <v>740</v>
       </c>
@@ -30687,8 +30909,9 @@
       <c r="AN218" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO218" s="4"/>
     </row>
-    <row r="219" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A219" s="12" t="s">
         <v>743</v>
       </c>
@@ -30795,8 +31018,9 @@
         <v>7702</v>
       </c>
       <c r="AN219" s="15"/>
+      <c r="AO219" s="4"/>
     </row>
-    <row r="220" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
         <v>746</v>
       </c>
@@ -30903,8 +31127,9 @@
         <v>1910</v>
       </c>
       <c r="AN220" s="11"/>
+      <c r="AO220" s="4"/>
     </row>
-    <row r="221" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A221" s="12" t="s">
         <v>749</v>
       </c>
@@ -31011,8 +31236,9 @@
         <v>9856</v>
       </c>
       <c r="AN221" s="15"/>
+      <c r="AO221" s="4"/>
     </row>
-    <row r="222" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A222" s="6" t="s">
         <v>753</v>
       </c>
@@ -31119,8 +31345,9 @@
         <v>80135</v>
       </c>
       <c r="AN222" s="11"/>
+      <c r="AO222" s="4"/>
     </row>
-    <row r="223" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A223" s="12" t="s">
         <v>756</v>
       </c>
@@ -31227,8 +31454,9 @@
         <v>136322</v>
       </c>
       <c r="AN223" s="15"/>
+      <c r="AO223" s="4"/>
     </row>
-    <row r="224" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A224" s="6" t="s">
         <v>759</v>
       </c>
@@ -31335,8 +31563,9 @@
         <v>1003589</v>
       </c>
       <c r="AN224" s="11"/>
+      <c r="AO224" s="4"/>
     </row>
-    <row r="225" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A225" s="12" t="s">
         <v>762</v>
       </c>
@@ -31445,8 +31674,9 @@
       <c r="AN225" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO225" s="4"/>
     </row>
-    <row r="226" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A226" s="6" t="s">
         <v>765</v>
       </c>
@@ -31555,8 +31785,9 @@
       <c r="AN226" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO226" s="4"/>
     </row>
-    <row r="227" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A227" s="12" t="s">
         <v>768</v>
       </c>
@@ -31665,8 +31896,9 @@
       <c r="AN227" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO227" s="4"/>
     </row>
-    <row r="228" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A228" s="6" t="s">
         <v>771</v>
       </c>
@@ -31775,8 +32007,9 @@
       <c r="AN228" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO228" s="4"/>
     </row>
-    <row r="229" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A229" s="12" t="s">
         <v>774</v>
       </c>
@@ -31883,8 +32116,9 @@
         <v>290</v>
       </c>
       <c r="AN229" s="15"/>
+      <c r="AO229" s="4"/>
     </row>
-    <row r="230" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A230" s="6" t="s">
         <v>777</v>
       </c>
@@ -31991,8 +32225,9 @@
         <v>50172</v>
       </c>
       <c r="AN230" s="11"/>
+      <c r="AO230" s="4"/>
     </row>
-    <row r="231" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A231" s="12" t="s">
         <v>780</v>
       </c>
@@ -32099,8 +32334,9 @@
         <v>115011</v>
       </c>
       <c r="AN231" s="15"/>
+      <c r="AO231" s="4"/>
     </row>
-    <row r="232" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A232" s="6" t="s">
         <v>783</v>
       </c>
@@ -32209,8 +32445,9 @@
       <c r="AN232" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO232" s="4"/>
     </row>
-    <row r="233" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A233" s="12" t="s">
         <v>786</v>
       </c>
@@ -32319,8 +32556,9 @@
       <c r="AN233" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO233" s="4"/>
     </row>
-    <row r="234" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A234" s="6" t="s">
         <v>788</v>
       </c>
@@ -32429,8 +32667,9 @@
       <c r="AN234" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO234" s="4"/>
     </row>
-    <row r="235" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A235" s="12" t="s">
         <v>791</v>
       </c>
@@ -32539,8 +32778,9 @@
       <c r="AN235" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO235" s="4"/>
     </row>
-    <row r="236" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A236" s="6" t="s">
         <v>794</v>
       </c>
@@ -32649,8 +32889,9 @@
       <c r="AN236" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO236" s="4"/>
     </row>
-    <row r="237" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A237" s="12" t="s">
         <v>797</v>
       </c>
@@ -32759,8 +33000,9 @@
       <c r="AN237" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO237" s="4"/>
     </row>
-    <row r="238" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A238" s="6" t="s">
         <v>800</v>
       </c>
@@ -32869,8 +33111,9 @@
       <c r="AN238" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO238" s="4"/>
     </row>
-    <row r="239" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A239" s="12" t="s">
         <v>804</v>
       </c>
@@ -32977,8 +33220,9 @@
         <v>8</v>
       </c>
       <c r="AN239" s="15"/>
+      <c r="AO239" s="4"/>
     </row>
-    <row r="240" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A240" s="6" t="s">
         <v>807</v>
       </c>
@@ -33085,8 +33329,9 @@
         <v>6848</v>
       </c>
       <c r="AN240" s="11"/>
+      <c r="AO240" s="4"/>
     </row>
-    <row r="241" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A241" s="12" t="s">
         <v>810</v>
       </c>
@@ -33193,8 +33438,9 @@
         <v>77917</v>
       </c>
       <c r="AN241" s="15"/>
+      <c r="AO241" s="4"/>
     </row>
-    <row r="242" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A242" s="6" t="s">
         <v>813</v>
       </c>
@@ -33301,8 +33547,9 @@
         <v>126046</v>
       </c>
       <c r="AN242" s="11"/>
+      <c r="AO242" s="4"/>
     </row>
-    <row r="243" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A243" s="12" t="s">
         <v>817</v>
       </c>
@@ -33409,8 +33656,9 @@
         <v>37960</v>
       </c>
       <c r="AN243" s="15"/>
+      <c r="AO243" s="4"/>
     </row>
-    <row r="244" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A244" s="6" t="s">
         <v>820</v>
       </c>
@@ -33517,8 +33765,9 @@
         <v>131973</v>
       </c>
       <c r="AN244" s="11"/>
+      <c r="AO244" s="4"/>
     </row>
-    <row r="245" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A245" s="12" t="s">
         <v>823</v>
       </c>
@@ -33625,8 +33874,9 @@
         <v>40045</v>
       </c>
       <c r="AN245" s="15"/>
+      <c r="AO245" s="4"/>
     </row>
-    <row r="246" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A246" s="6" t="s">
         <v>826</v>
       </c>
@@ -33735,8 +33985,9 @@
       <c r="AN246" s="11" t="s">
         <v>830</v>
       </c>
+      <c r="AO246" s="4"/>
     </row>
-    <row r="247" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A247" s="12" t="s">
         <v>831</v>
       </c>
@@ -33843,8 +34094,9 @@
         <v>1948</v>
       </c>
       <c r="AN247" s="15"/>
+      <c r="AO247" s="4"/>
     </row>
-    <row r="248" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A248" s="6" t="s">
         <v>835</v>
       </c>
@@ -33953,8 +34205,9 @@
       <c r="AN248" s="45" t="s">
         <v>838</v>
       </c>
+      <c r="AO248" s="4"/>
     </row>
-    <row r="249" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A249" s="12" t="s">
         <v>839</v>
       </c>
@@ -34061,8 +34314,9 @@
         <v>15336</v>
       </c>
       <c r="AN249" s="15"/>
+      <c r="AO249" s="4"/>
     </row>
-    <row r="250" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A250" s="6" t="s">
         <v>842</v>
       </c>
@@ -34169,8 +34423,9 @@
         <v>51193</v>
       </c>
       <c r="AN250" s="11"/>
+      <c r="AO250" s="4"/>
     </row>
-    <row r="251" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A251" s="12" t="s">
         <v>845</v>
       </c>
@@ -34279,8 +34534,9 @@
       <c r="AN251" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO251" s="4"/>
     </row>
-    <row r="252" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A252" s="6" t="s">
         <v>848</v>
       </c>
@@ -34389,8 +34645,9 @@
       <c r="AN252" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO252" s="4"/>
     </row>
-    <row r="253" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A253" s="12" t="s">
         <v>850</v>
       </c>
@@ -34499,8 +34756,9 @@
       <c r="AN253" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO253" s="4"/>
     </row>
-    <row r="254" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A254" s="6" t="s">
         <v>852</v>
       </c>
@@ -34607,8 +34865,9 @@
         <v>64</v>
       </c>
       <c r="AN254" s="11"/>
+      <c r="AO254" s="4"/>
     </row>
-    <row r="255" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A255" s="12" t="s">
         <v>855</v>
       </c>
@@ -34717,8 +34976,9 @@
       <c r="AN255" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO255" s="4"/>
     </row>
-    <row r="256" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A256" s="6" t="s">
         <v>858</v>
       </c>
@@ -34825,8 +35085,9 @@
         <v>0</v>
       </c>
       <c r="AN256" s="11"/>
+      <c r="AO256" s="4"/>
     </row>
-    <row r="257" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A257" s="12" t="s">
         <v>862</v>
       </c>
@@ -34935,8 +35196,9 @@
       <c r="AN257" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO257" s="4"/>
     </row>
-    <row r="258" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A258" s="6" t="s">
         <v>864</v>
       </c>
@@ -35045,8 +35307,9 @@
       <c r="AN258" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO258" s="4"/>
     </row>
-    <row r="259" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A259" s="12" t="s">
         <v>867</v>
       </c>
@@ -35155,8 +35418,9 @@
       <c r="AN259" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO259" s="4"/>
     </row>
-    <row r="260" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A260" s="6" t="s">
         <v>870</v>
       </c>
@@ -35263,8 +35527,9 @@
         <v>1480</v>
       </c>
       <c r="AN260" s="11"/>
+      <c r="AO260" s="4"/>
     </row>
-    <row r="261" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A261" s="12" t="s">
         <v>874</v>
       </c>
@@ -35373,8 +35638,9 @@
       <c r="AN261" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO261" s="4"/>
     </row>
-    <row r="262" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A262" s="6" t="s">
         <v>878</v>
       </c>
@@ -35481,8 +35747,9 @@
         <v>142</v>
       </c>
       <c r="AN262" s="11"/>
+      <c r="AO262" s="4"/>
     </row>
-    <row r="263" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A263" s="12" t="s">
         <v>881</v>
       </c>
@@ -35591,8 +35858,9 @@
       <c r="AN263" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO263" s="4"/>
     </row>
-    <row r="264" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A264" s="6" t="s">
         <v>884</v>
       </c>
@@ -35701,8 +35969,9 @@
       <c r="AN264" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO264" s="4"/>
     </row>
-    <row r="265" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A265" s="12" t="s">
         <v>887</v>
       </c>
@@ -35811,8 +36080,9 @@
       <c r="AN265" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO265" s="4"/>
     </row>
-    <row r="266" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A266" s="6" t="s">
         <v>890</v>
       </c>
@@ -35921,8 +36191,9 @@
       <c r="AN266" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO266" s="4"/>
     </row>
-    <row r="267" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A267" s="12" t="s">
         <v>893</v>
       </c>
@@ -36029,8 +36300,9 @@
         <v>7357</v>
       </c>
       <c r="AN267" s="15"/>
+      <c r="AO267" s="4"/>
     </row>
-    <row r="268" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A268" s="6" t="s">
         <v>895</v>
       </c>
@@ -36139,8 +36411,9 @@
       <c r="AN268" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO268" s="4"/>
     </row>
-    <row r="269" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A269" s="12" t="s">
         <v>898</v>
       </c>
@@ -36249,8 +36522,9 @@
       <c r="AN269" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO269" s="4"/>
     </row>
-    <row r="270" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A270" s="6" t="s">
         <v>901</v>
       </c>
@@ -36359,8 +36633,9 @@
       <c r="AN270" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO270" s="4"/>
     </row>
-    <row r="271" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A271" s="12" t="s">
         <v>903</v>
       </c>
@@ -36469,8 +36744,9 @@
       <c r="AN271" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO271" s="4"/>
     </row>
-    <row r="272" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A272" s="6" t="s">
         <v>907</v>
       </c>
@@ -36579,8 +36855,9 @@
       <c r="AN272" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO272" s="4"/>
     </row>
-    <row r="273" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A273" s="12" t="s">
         <v>911</v>
       </c>
@@ -36689,8 +36966,9 @@
       <c r="AN273" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO273" s="4"/>
     </row>
-    <row r="274" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A274" s="6" t="s">
         <v>915</v>
       </c>
@@ -36799,8 +37077,9 @@
       <c r="AN274" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO274" s="4"/>
     </row>
-    <row r="275" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A275" s="12" t="s">
         <v>918</v>
       </c>
@@ -36907,8 +37186,9 @@
         <v>112908</v>
       </c>
       <c r="AN275" s="15"/>
+      <c r="AO275" s="4"/>
     </row>
-    <row r="276" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A276" s="6" t="s">
         <v>921</v>
       </c>
@@ -37017,8 +37297,9 @@
       <c r="AN276" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO276" s="4"/>
     </row>
-    <row r="277" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A277" s="12" t="s">
         <v>925</v>
       </c>
@@ -37125,8 +37406,9 @@
         <v>576</v>
       </c>
       <c r="AN277" s="15"/>
+      <c r="AO277" s="4"/>
     </row>
-    <row r="278" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A278" s="6" t="s">
         <v>929</v>
       </c>
@@ -37233,8 +37515,9 @@
         <v>450</v>
       </c>
       <c r="AN278" s="11"/>
+      <c r="AO278" s="4"/>
     </row>
-    <row r="279" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A279" s="12" t="s">
         <v>934</v>
       </c>
@@ -37343,8 +37626,9 @@
       <c r="AN279" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO279" s="4"/>
     </row>
-    <row r="280" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A280" s="6" t="s">
         <v>938</v>
       </c>
@@ -37451,8 +37735,9 @@
         <v>2048</v>
       </c>
       <c r="AN280" s="11"/>
+      <c r="AO280" s="4"/>
     </row>
-    <row r="281" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A281" s="12" t="s">
         <v>941</v>
       </c>
@@ -37559,8 +37844,9 @@
         <v>21740</v>
       </c>
       <c r="AN281" s="15"/>
+      <c r="AO281" s="4"/>
     </row>
-    <row r="282" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A282" s="6" t="s">
         <v>944</v>
       </c>
@@ -37667,8 +37953,9 @@
         <v>6570</v>
       </c>
       <c r="AN282" s="11"/>
+      <c r="AO282" s="4"/>
     </row>
-    <row r="283" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A283" s="12" t="s">
         <v>947</v>
       </c>
@@ -37775,8 +38062,9 @@
         <v>79180</v>
       </c>
       <c r="AN283" s="15"/>
+      <c r="AO283" s="4"/>
     </row>
-    <row r="284" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A284" s="6" t="s">
         <v>950</v>
       </c>
@@ -37883,8 +38171,9 @@
         <v>13589</v>
       </c>
       <c r="AN284" s="11"/>
+      <c r="AO284" s="4"/>
     </row>
-    <row r="285" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A285" s="12" t="s">
         <v>954</v>
       </c>
@@ -37991,8 +38280,9 @@
         <v>2</v>
       </c>
       <c r="AN285" s="15"/>
+      <c r="AO285" s="4"/>
     </row>
-    <row r="286" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A286" s="6" t="s">
         <v>957</v>
       </c>
@@ -38099,8 +38389,9 @@
         <v>0</v>
       </c>
       <c r="AN286" s="11"/>
+      <c r="AO286" s="4"/>
     </row>
-    <row r="287" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A287" s="12" t="s">
         <v>961</v>
       </c>
@@ -38207,8 +38498,9 @@
         <v>2</v>
       </c>
       <c r="AN287" s="15"/>
+      <c r="AO287" s="4"/>
     </row>
-    <row r="288" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A288" s="6" t="s">
         <v>965</v>
       </c>
@@ -38315,8 +38607,9 @@
         <v>552</v>
       </c>
       <c r="AN288" s="11"/>
+      <c r="AO288" s="4"/>
     </row>
-    <row r="289" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A289" s="12" t="s">
         <v>968</v>
       </c>
@@ -38423,8 +38716,9 @@
         <v>200</v>
       </c>
       <c r="AN289" s="15"/>
+      <c r="AO289" s="4"/>
     </row>
-    <row r="290" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A290" s="6" t="s">
         <v>972</v>
       </c>
@@ -38531,8 +38825,9 @@
         <v>364</v>
       </c>
       <c r="AN290" s="11"/>
+      <c r="AO290" s="4"/>
     </row>
-    <row r="291" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A291" s="12" t="s">
         <v>975</v>
       </c>
@@ -38639,8 +38934,9 @@
         <v>5685</v>
       </c>
       <c r="AN291" s="15"/>
+      <c r="AO291" s="4"/>
     </row>
-    <row r="292" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A292" s="6" t="s">
         <v>978</v>
       </c>
@@ -38747,8 +39043,9 @@
         <v>67138</v>
       </c>
       <c r="AN292" s="11"/>
+      <c r="AO292" s="4"/>
     </row>
-    <row r="293" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A293" s="12" t="s">
         <v>981</v>
       </c>
@@ -38855,8 +39152,9 @@
         <v>160377</v>
       </c>
       <c r="AN293" s="15"/>
+      <c r="AO293" s="4"/>
     </row>
-    <row r="294" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A294" s="6" t="s">
         <v>984</v>
       </c>
@@ -38965,8 +39263,9 @@
       <c r="AN294" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO294" s="4"/>
     </row>
-    <row r="295" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A295" s="12" t="s">
         <v>986</v>
       </c>
@@ -39075,8 +39374,9 @@
       <c r="AN295" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO295" s="4"/>
     </row>
-    <row r="296" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A296" s="6" t="s">
         <v>989</v>
       </c>
@@ -39183,8 +39483,9 @@
         <v>25426</v>
       </c>
       <c r="AN296" s="11"/>
+      <c r="AO296" s="4"/>
     </row>
-    <row r="297" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A297" s="12" t="s">
         <v>992</v>
       </c>
@@ -39293,8 +39594,9 @@
       <c r="AN297" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO297" s="4"/>
     </row>
-    <row r="298" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A298" s="6" t="s">
         <v>995</v>
       </c>
@@ -39403,8 +39705,9 @@
       <c r="AN298" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO298" s="4"/>
     </row>
-    <row r="299" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A299" s="12" t="s">
         <v>997</v>
       </c>
@@ -39513,8 +39816,9 @@
       <c r="AN299" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO299" s="4"/>
     </row>
-    <row r="300" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A300" s="6" t="s">
         <v>999</v>
       </c>
@@ -39621,8 +39925,9 @@
         <v>4914</v>
       </c>
       <c r="AN300" s="11"/>
+      <c r="AO300" s="4"/>
     </row>
-    <row r="301" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A301" s="12" t="s">
         <v>1002</v>
       </c>
@@ -39729,8 +40034,9 @@
         <v>2086</v>
       </c>
       <c r="AN301" s="15"/>
+      <c r="AO301" s="4"/>
     </row>
-    <row r="302" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A302" s="6" t="s">
         <v>1005</v>
       </c>
@@ -39837,8 +40143,9 @@
         <v>97991</v>
       </c>
       <c r="AN302" s="11"/>
+      <c r="AO302" s="4"/>
     </row>
-    <row r="303" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A303" s="12" t="s">
         <v>1009</v>
       </c>
@@ -39945,8 +40252,9 @@
         <v>38037</v>
       </c>
       <c r="AN303" s="15"/>
+      <c r="AO303" s="4"/>
     </row>
-    <row r="304" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A304" s="6" t="s">
         <v>1012</v>
       </c>
@@ -40053,8 +40361,9 @@
         <v>190</v>
       </c>
       <c r="AN304" s="11"/>
+      <c r="AO304" s="4"/>
     </row>
-    <row r="305" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A305" s="12" t="s">
         <v>1015</v>
       </c>
@@ -40163,8 +40472,9 @@
       <c r="AN305" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO305" s="4"/>
     </row>
-    <row r="306" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A306" s="6" t="s">
         <v>1018</v>
       </c>
@@ -40271,8 +40581,9 @@
         <v>582</v>
       </c>
       <c r="AN306" s="11"/>
+      <c r="AO306" s="4"/>
     </row>
-    <row r="307" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A307" s="12" t="s">
         <v>1021</v>
       </c>
@@ -40379,8 +40690,9 @@
         <v>10546</v>
       </c>
       <c r="AN307" s="15"/>
+      <c r="AO307" s="4"/>
     </row>
-    <row r="308" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A308" s="6" t="s">
         <v>1024</v>
       </c>
@@ -40487,8 +40799,9 @@
         <v>40745</v>
       </c>
       <c r="AN308" s="11"/>
+      <c r="AO308" s="4"/>
     </row>
-    <row r="309" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A309" s="12" t="s">
         <v>1027</v>
       </c>
@@ -40597,8 +40910,9 @@
       <c r="AN309" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO309" s="4"/>
     </row>
-    <row r="310" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A310" s="6" t="s">
         <v>1030</v>
       </c>
@@ -40707,8 +41021,9 @@
       <c r="AN310" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO310" s="4"/>
     </row>
-    <row r="311" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A311" s="12" t="s">
         <v>1033</v>
       </c>
@@ -40825,8 +41140,9 @@
       <c r="AN311" s="15" t="s">
         <v>1036</v>
       </c>
+      <c r="AO311" s="4"/>
     </row>
-    <row r="312" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A312" s="6" t="s">
         <v>1037</v>
       </c>
@@ -40935,8 +41251,9 @@
       <c r="AN312" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO312" s="4"/>
     </row>
-    <row r="313" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A313" s="12" t="s">
         <v>1041</v>
       </c>
@@ -41045,8 +41362,9 @@
       <c r="AN313" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO313" s="4"/>
     </row>
-    <row r="314" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A314" s="6" t="s">
         <v>1044</v>
       </c>
@@ -41153,8 +41471,9 @@
         <v>4</v>
       </c>
       <c r="AN314" s="11"/>
+      <c r="AO314" s="4"/>
     </row>
-    <row r="315" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A315" s="12" t="s">
         <v>1048</v>
       </c>
@@ -41261,8 +41580,9 @@
         <v>30540</v>
       </c>
       <c r="AN315" s="15"/>
+      <c r="AO315" s="4"/>
     </row>
-    <row r="316" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A316" s="6" t="s">
         <v>1052</v>
       </c>
@@ -41369,8 +41689,9 @@
         <v>10118</v>
       </c>
       <c r="AN316" s="11"/>
+      <c r="AO316" s="4"/>
     </row>
-    <row r="317" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A317" s="12" t="s">
         <v>1056</v>
       </c>
@@ -41477,8 +41798,9 @@
         <v>442204</v>
       </c>
       <c r="AN317" s="15"/>
+      <c r="AO317" s="4"/>
     </row>
-    <row r="318" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A318" s="6" t="s">
         <v>1059</v>
       </c>
@@ -41585,8 +41907,9 @@
         <v>18542</v>
       </c>
       <c r="AN318" s="11"/>
+      <c r="AO318" s="4"/>
     </row>
-    <row r="319" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A319" s="12" t="s">
         <v>1062</v>
       </c>
@@ -41693,8 +42016,9 @@
         <v>51448</v>
       </c>
       <c r="AN319" s="15"/>
+      <c r="AO319" s="4"/>
     </row>
-    <row r="320" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A320" s="6" t="s">
         <v>1065</v>
       </c>
@@ -41801,8 +42125,9 @@
         <v>3937</v>
       </c>
       <c r="AN320" s="11"/>
+      <c r="AO320" s="4"/>
     </row>
-    <row r="321" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A321" s="12" t="s">
         <v>1068</v>
       </c>
@@ -41909,8 +42234,9 @@
         <v>13116</v>
       </c>
       <c r="AN321" s="15"/>
+      <c r="AO321" s="4"/>
     </row>
-    <row r="322" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A322" s="6" t="s">
         <v>1070</v>
       </c>
@@ -42017,8 +42343,9 @@
         <v>45312</v>
       </c>
       <c r="AN322" s="11"/>
+      <c r="AO322" s="4"/>
     </row>
-    <row r="323" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A323" s="12" t="s">
         <v>1073</v>
       </c>
@@ -42125,8 +42452,9 @@
         <v>7394</v>
       </c>
       <c r="AN323" s="15"/>
+      <c r="AO323" s="4"/>
     </row>
-    <row r="324" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A324" s="6" t="s">
         <v>1076</v>
       </c>
@@ -42233,8 +42561,9 @@
         <v>132009</v>
       </c>
       <c r="AN324" s="11"/>
+      <c r="AO324" s="4"/>
     </row>
-    <row r="325" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A325" s="12" t="s">
         <v>1079</v>
       </c>
@@ -42341,8 +42670,9 @@
         <v>184</v>
       </c>
       <c r="AN325" s="15"/>
+      <c r="AO325" s="4"/>
     </row>
-    <row r="326" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A326" s="6" t="s">
         <v>1083</v>
       </c>
@@ -42449,8 +42779,9 @@
         <v>4242</v>
       </c>
       <c r="AN326" s="11"/>
+      <c r="AO326" s="4"/>
     </row>
-    <row r="327" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A327" s="12" t="s">
         <v>1087</v>
       </c>
@@ -42557,8 +42888,9 @@
         <v>166</v>
       </c>
       <c r="AN327" s="15"/>
+      <c r="AO327" s="4"/>
     </row>
-    <row r="328" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A328" s="6" t="s">
         <v>1091</v>
       </c>
@@ -42665,8 +42997,9 @@
         <v>45872</v>
       </c>
       <c r="AN328" s="11"/>
+      <c r="AO328" s="4"/>
     </row>
-    <row r="329" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A329" s="12" t="s">
         <v>1093</v>
       </c>
@@ -42773,8 +43106,9 @@
         <v>144</v>
       </c>
       <c r="AN329" s="15"/>
+      <c r="AO329" s="4"/>
     </row>
-    <row r="330" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A330" s="6" t="s">
         <v>1095</v>
       </c>
@@ -42881,8 +43215,9 @@
         <v>26</v>
       </c>
       <c r="AN330" s="11"/>
+      <c r="AO330" s="4"/>
     </row>
-    <row r="331" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A331" s="12" t="s">
         <v>1098</v>
       </c>
@@ -42989,8 +43324,9 @@
         <v>2</v>
       </c>
       <c r="AN331" s="15"/>
+      <c r="AO331" s="4"/>
     </row>
-    <row r="332" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A332" s="6" t="s">
         <v>1100</v>
       </c>
@@ -43097,8 +43433,9 @@
         <v>196</v>
       </c>
       <c r="AN332" s="11"/>
+      <c r="AO332" s="4"/>
     </row>
-    <row r="333" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A333" s="12" t="s">
         <v>1103</v>
       </c>
@@ -43205,8 +43542,9 @@
         <v>154</v>
       </c>
       <c r="AN333" s="15"/>
+      <c r="AO333" s="4"/>
     </row>
-    <row r="334" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A334" s="6" t="s">
         <v>1105</v>
       </c>
@@ -43313,8 +43651,9 @@
         <v>484</v>
       </c>
       <c r="AN334" s="11"/>
+      <c r="AO334" s="4"/>
     </row>
-    <row r="335" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A335" s="12" t="s">
         <v>1108</v>
       </c>
@@ -43421,8 +43760,9 @@
         <v>5205</v>
       </c>
       <c r="AN335" s="15"/>
+      <c r="AO335" s="4"/>
     </row>
-    <row r="336" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A336" s="6" t="s">
         <v>1111</v>
       </c>
@@ -43529,8 +43869,9 @@
         <v>25659</v>
       </c>
       <c r="AN336" s="11"/>
+      <c r="AO336" s="4"/>
     </row>
-    <row r="337" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A337" s="12" t="s">
         <v>1113</v>
       </c>
@@ -43637,8 +43978,9 @@
         <v>14</v>
       </c>
       <c r="AN337" s="15"/>
+      <c r="AO337" s="4"/>
     </row>
-    <row r="338" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A338" s="6" t="s">
         <v>1115</v>
       </c>
@@ -43745,8 +44087,9 @@
         <v>22883</v>
       </c>
       <c r="AN338" s="11"/>
+      <c r="AO338" s="4"/>
     </row>
-    <row r="339" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A339" s="12" t="s">
         <v>1118</v>
       </c>
@@ -43853,8 +44196,9 @@
         <v>23175</v>
       </c>
       <c r="AN339" s="15"/>
+      <c r="AO339" s="4"/>
     </row>
-    <row r="340" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A340" s="6" t="s">
         <v>1121</v>
       </c>
@@ -43961,8 +44305,9 @@
         <v>103395</v>
       </c>
       <c r="AN340" s="11"/>
+      <c r="AO340" s="4"/>
     </row>
-    <row r="341" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A341" s="12" t="s">
         <v>1124</v>
       </c>
@@ -44069,8 +44414,9 @@
         <v>85726</v>
       </c>
       <c r="AN341" s="15"/>
+      <c r="AO341" s="4"/>
     </row>
-    <row r="342" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A342" s="6" t="s">
         <v>1127</v>
       </c>
@@ -44177,8 +44523,9 @@
         <v>53078</v>
       </c>
       <c r="AN342" s="11"/>
+      <c r="AO342" s="4"/>
     </row>
-    <row r="343" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A343" s="12" t="s">
         <v>1130</v>
       </c>
@@ -44285,8 +44632,9 @@
         <v>22</v>
       </c>
       <c r="AN343" s="15"/>
+      <c r="AO343" s="4"/>
     </row>
-    <row r="344" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A344" s="6" t="s">
         <v>1132</v>
       </c>
@@ -44393,8 +44741,9 @@
         <v>872</v>
       </c>
       <c r="AN344" s="11"/>
+      <c r="AO344" s="4"/>
     </row>
-    <row r="345" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A345" s="12" t="s">
         <v>1135</v>
       </c>
@@ -44501,8 +44850,9 @@
         <v>58492</v>
       </c>
       <c r="AN345" s="15"/>
+      <c r="AO345" s="4"/>
     </row>
-    <row r="346" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A346" s="6" t="s">
         <v>1138</v>
       </c>
@@ -44609,8 +44959,9 @@
         <v>104242</v>
       </c>
       <c r="AN346" s="11"/>
+      <c r="AO346" s="4"/>
     </row>
-    <row r="347" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A347" s="12" t="s">
         <v>1141</v>
       </c>
@@ -44717,8 +45068,9 @@
         <v>4813</v>
       </c>
       <c r="AN347" s="15"/>
+      <c r="AO347" s="4"/>
     </row>
-    <row r="348" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A348" s="6" t="s">
         <v>1144</v>
       </c>
@@ -44825,8 +45177,9 @@
         <v>15214</v>
       </c>
       <c r="AN348" s="11"/>
+      <c r="AO348" s="4"/>
     </row>
-    <row r="349" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A349" s="12" t="s">
         <v>1147</v>
       </c>
@@ -44933,8 +45286,9 @@
         <v>23449</v>
       </c>
       <c r="AN349" s="15"/>
+      <c r="AO349" s="4"/>
     </row>
-    <row r="350" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A350" s="6" t="s">
         <v>1150</v>
       </c>
@@ -45041,8 +45395,9 @@
         <v>6033</v>
       </c>
       <c r="AN350" s="11"/>
+      <c r="AO350" s="4"/>
     </row>
-    <row r="351" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A351" s="12" t="s">
         <v>1153</v>
       </c>
@@ -45149,8 +45504,9 @@
         <v>5597</v>
       </c>
       <c r="AN351" s="15"/>
+      <c r="AO351" s="4"/>
     </row>
-    <row r="352" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A352" s="6" t="s">
         <v>1156</v>
       </c>
@@ -45257,8 +45613,9 @@
         <v>1374840</v>
       </c>
       <c r="AN352" s="11"/>
+      <c r="AO352" s="4"/>
     </row>
-    <row r="353" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A353" s="12" t="s">
         <v>1160</v>
       </c>
@@ -45367,8 +45724,9 @@
       <c r="AN353" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO353" s="4"/>
     </row>
-    <row r="354" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A354" s="6" t="s">
         <v>1162</v>
       </c>
@@ -45477,8 +45835,9 @@
       <c r="AN354" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO354" s="4"/>
     </row>
-    <row r="355" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A355" s="12" t="s">
         <v>1166</v>
       </c>
@@ -45585,8 +45944,9 @@
         <v>44</v>
       </c>
       <c r="AN355" s="15"/>
+      <c r="AO355" s="4"/>
     </row>
-    <row r="356" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A356" s="6" t="s">
         <v>1168</v>
       </c>
@@ -45693,8 +46053,9 @@
         <v>2</v>
       </c>
       <c r="AN356" s="11"/>
+      <c r="AO356" s="4"/>
     </row>
-    <row r="357" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A357" s="12" t="s">
         <v>1170</v>
       </c>
@@ -45801,8 +46162,9 @@
         <v>11339</v>
       </c>
       <c r="AN357" s="15"/>
+      <c r="AO357" s="4"/>
     </row>
-    <row r="358" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A358" s="6" t="s">
         <v>1174</v>
       </c>
@@ -45909,8 +46271,9 @@
         <v>5332</v>
       </c>
       <c r="AN358" s="11"/>
+      <c r="AO358" s="4"/>
     </row>
-    <row r="359" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A359" s="12" t="s">
         <v>1177</v>
       </c>
@@ -46017,8 +46380,9 @@
         <v>284</v>
       </c>
       <c r="AN359" s="15"/>
+      <c r="AO359" s="4"/>
     </row>
-    <row r="360" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A360" s="6" t="s">
         <v>1180</v>
       </c>
@@ -46125,8 +46489,9 @@
         <v>24</v>
       </c>
       <c r="AN360" s="11"/>
+      <c r="AO360" s="4"/>
     </row>
-    <row r="361" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A361" s="12" t="s">
         <v>1183</v>
       </c>
@@ -46233,8 +46598,9 @@
         <v>191794</v>
       </c>
       <c r="AN361" s="15"/>
+      <c r="AO361" s="4"/>
     </row>
-    <row r="362" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A362" s="6" t="s">
         <v>1187</v>
       </c>
@@ -46343,8 +46709,9 @@
       <c r="AN362" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO362" s="4"/>
     </row>
-    <row r="363" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A363" s="12" t="s">
         <v>1190</v>
       </c>
@@ -46451,8 +46818,9 @@
         <v>6767</v>
       </c>
       <c r="AN363" s="15"/>
+      <c r="AO363" s="4"/>
     </row>
-    <row r="364" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A364" s="6" t="s">
         <v>1194</v>
       </c>
@@ -46559,8 +46927,9 @@
         <v>626</v>
       </c>
       <c r="AN364" s="11"/>
+      <c r="AO364" s="4"/>
     </row>
-    <row r="365" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A365" s="12" t="s">
         <v>1197</v>
       </c>
@@ -46667,8 +47036,9 @@
         <v>204</v>
       </c>
       <c r="AN365" s="15"/>
+      <c r="AO365" s="4"/>
     </row>
-    <row r="366" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A366" s="6" t="s">
         <v>1201</v>
       </c>
@@ -46777,8 +47147,9 @@
       <c r="AN366" s="11" t="s">
         <v>71</v>
       </c>
+      <c r="AO366" s="4"/>
     </row>
-    <row r="367" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A367" s="12" t="s">
         <v>1204</v>
       </c>
@@ -46887,8 +47258,9 @@
       <c r="AN367" s="15" t="s">
         <v>71</v>
       </c>
+      <c r="AO367" s="4"/>
     </row>
-    <row r="368" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A368" s="6" t="s">
         <v>1207</v>
       </c>
@@ -46995,8 +47367,9 @@
         <v>1216</v>
       </c>
       <c r="AN368" s="11"/>
+      <c r="AO368" s="4"/>
     </row>
-    <row r="369" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A369" s="12" t="s">
         <v>1210</v>
       </c>
@@ -47103,8 +47476,9 @@
         <v>64531</v>
       </c>
       <c r="AN369" s="15"/>
+      <c r="AO369" s="4"/>
     </row>
-    <row r="370" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A370" s="6" t="s">
         <v>1213</v>
       </c>
@@ -47211,8 +47585,9 @@
         <v>92644</v>
       </c>
       <c r="AN370" s="11"/>
+      <c r="AO370" s="4"/>
     </row>
-    <row r="371" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A371" s="12" t="s">
         <v>1216</v>
       </c>
@@ -47319,8 +47694,9 @@
         <v>382336</v>
       </c>
       <c r="AN371" s="15"/>
+      <c r="AO371" s="4"/>
     </row>
-    <row r="372" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A372" s="6" t="s">
         <v>1219</v>
       </c>
@@ -47427,8 +47803,9 @@
         <v>0</v>
       </c>
       <c r="AN372" s="11"/>
+      <c r="AO372" s="4"/>
     </row>
-    <row r="373" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A373" s="12" t="s">
         <v>1223</v>
       </c>
@@ -47535,8 +47912,9 @@
         <v>37105</v>
       </c>
       <c r="AN373" s="15"/>
+      <c r="AO373" s="4"/>
     </row>
-    <row r="374" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A374" s="6" t="s">
         <v>1227</v>
       </c>
@@ -47643,8 +48021,9 @@
         <v>219361</v>
       </c>
       <c r="AN374" s="11"/>
+      <c r="AO374" s="4"/>
     </row>
-    <row r="375" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A375" s="12" t="s">
         <v>1230</v>
       </c>
@@ -47751,8 +48130,9 @@
         <v>17016</v>
       </c>
       <c r="AN375" s="15"/>
+      <c r="AO375" s="4"/>
     </row>
-    <row r="376" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A376" s="6" t="s">
         <v>1233</v>
       </c>
@@ -47859,8 +48239,9 @@
         <v>122</v>
       </c>
       <c r="AN376" s="11"/>
+      <c r="AO376" s="4"/>
     </row>
-    <row r="377" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A377" s="12" t="s">
         <v>1235</v>
       </c>
@@ -47967,8 +48348,9 @@
         <v>1338</v>
       </c>
       <c r="AN377" s="15"/>
+      <c r="AO377" s="4"/>
     </row>
-    <row r="378" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A378" s="6" t="s">
         <v>1238</v>
       </c>
@@ -48075,8 +48457,9 @@
         <v>222646</v>
       </c>
       <c r="AN378" s="11"/>
+      <c r="AO378" s="4"/>
     </row>
-    <row r="379" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A379" s="12" t="s">
         <v>1240</v>
       </c>
@@ -48183,8 +48566,9 @@
         <v>3842</v>
       </c>
       <c r="AN379" s="15"/>
+      <c r="AO379" s="4"/>
     </row>
-    <row r="380" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A380" s="6" t="s">
         <v>1242</v>
       </c>
@@ -48291,8 +48675,9 @@
         <v>0</v>
       </c>
       <c r="AN380" s="11"/>
+      <c r="AO380" s="4"/>
     </row>
-    <row r="381" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A381" s="12" t="s">
         <v>1245</v>
       </c>
@@ -48399,8 +48784,9 @@
         <v>4314</v>
       </c>
       <c r="AN381" s="15"/>
+      <c r="AO381" s="4"/>
     </row>
-    <row r="382" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="382" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A382" s="6" t="s">
         <v>1249</v>
       </c>
@@ -48507,8 +48893,9 @@
         <v>54709</v>
       </c>
       <c r="AN382" s="11"/>
+      <c r="AO382" s="4"/>
     </row>
-    <row r="383" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="383" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A383" s="12" t="s">
         <v>1252</v>
       </c>
@@ -48615,8 +49002,9 @@
         <v>76961</v>
       </c>
       <c r="AN383" s="15"/>
+      <c r="AO383" s="4"/>
     </row>
-    <row r="384" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A384" s="6" t="s">
         <v>1254</v>
       </c>
@@ -48723,8 +49111,9 @@
         <v>102124</v>
       </c>
       <c r="AN384" s="11"/>
+      <c r="AO384" s="4"/>
     </row>
-    <row r="385" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A385" s="12" t="s">
         <v>1257</v>
       </c>
@@ -48831,8 +49220,9 @@
         <v>319581</v>
       </c>
       <c r="AN385" s="15"/>
+      <c r="AO385" s="4"/>
     </row>
-    <row r="386" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A386" s="6" t="s">
         <v>1261</v>
       </c>
@@ -48939,8 +49329,9 @@
         <v>1566</v>
       </c>
       <c r="AN386" s="11"/>
+      <c r="AO386" s="4"/>
     </row>
-    <row r="387" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A387" s="12" t="s">
         <v>1263</v>
       </c>
@@ -49049,8 +49440,9 @@
         <v>17294</v>
       </c>
       <c r="AN387" s="15"/>
+      <c r="AO387" s="4"/>
     </row>
-    <row r="388" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A388" s="18" t="s">
         <v>1269</v>
       </c>
@@ -49157,8 +49549,9 @@
         <v>14137</v>
       </c>
       <c r="AN388" s="23"/>
+      <c r="AO388" s="4"/>
     </row>
-    <row r="389" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A389" s="4"/>
       <c r="B389" s="4"/>
       <c r="C389" s="4"/>
@@ -49199,8 +49592,9 @@
       <c r="AL389" s="47"/>
       <c r="AM389" s="47"/>
       <c r="AN389" s="4"/>
+      <c r="AO389" s="4"/>
     </row>
-    <row r="390" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A390" s="4"/>
       <c r="B390" s="4"/>
       <c r="C390" s="4"/>
@@ -49241,6 +49635,7 @@
       <c r="AL390" s="47"/>
       <c r="AM390" s="47"/>
       <c r="AN390" s="4"/>
+      <c r="AO390" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -50329,6 +50724,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="2624f4f0-6830-48b6-9c21-80b2613400ca" xsi:nil="true"/>
@@ -50337,15 +50741,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -50580,20 +50975,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0E9CFC5-E3D9-4ED1-BD0E-6DB50CB80DD6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15821E26-0416-43DF-8894-FB2498CD7580}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="2624f4f0-6830-48b6-9c21-80b2613400ca"/>
     <ds:schemaRef ds:uri="d337210d-25f7-4ced-91e1-19a0946fcb25"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0E9CFC5-E3D9-4ED1-BD0E-6DB50CB80DD6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>